<commit_message>
Added the valueset section IG
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-Account.xlsx
+++ b/output/StructureDefinition-Account.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$32</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="213">
   <si>
     <t>Path</t>
   </si>
@@ -150,9 +150,6 @@
     <t>A financial tool for tracking value accrued for a particular purpose.  In the healthcare field, used to track charges for a patient, cost centers, etc.</t>
   </si>
   <si>
-    <t>DomainResource</t>
-  </si>
-  <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
 dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
@@ -321,16 +318,6 @@
     <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
   </si>
   <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>DomainResource.extension</t>
   </si>
   <si>
@@ -352,6 +339,147 @@
   </si>
   <si>
     <t>DomainResource.modifierExtension</t>
+  </si>
+  <si>
+    <t>Account.identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier
+</t>
+  </si>
+  <si>
+    <t>Account number</t>
+  </si>
+  <si>
+    <t>Unique identifier used to reference the account.  Might or might not be intended for human use (e.g. credit card number).</t>
+  </si>
+  <si>
+    <t>.id</t>
+  </si>
+  <si>
+    <t>FiveWs.identifier</t>
+  </si>
+  <si>
+    <t>Account.status</t>
+  </si>
+  <si>
+    <t>active | inactive | entered-in-error | on-hold | unknown</t>
+  </si>
+  <si>
+    <t>Indicates whether the account is presently used/usable or not.</t>
+  </si>
+  <si>
+    <t>This element is labeled as a modifier because the status contains the codes inactive and entered-in-error that mark the Account as not currently valid.</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>Indicates whether the account is available to be used.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/account-status|4.0.1</t>
+  </si>
+  <si>
+    <t>.statusCode</t>
+  </si>
+  <si>
+    <t>FiveWs.status</t>
+  </si>
+  <si>
+    <t>Account.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CodeableConcept
+</t>
+  </si>
+  <si>
+    <t>E.g. patient, expense, depreciation</t>
+  </si>
+  <si>
+    <t>Categorizes the account for reporting and searching purposes.</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>The usage type of this account, permits categorization of accounts.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/account-type</t>
+  </si>
+  <si>
+    <t>.code</t>
+  </si>
+  <si>
+    <t>FiveWs.class</t>
+  </si>
+  <si>
+    <t>Account.name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title
+</t>
+  </si>
+  <si>
+    <t>Human-readable label</t>
+  </si>
+  <si>
+    <t>Name used for the account when displaying it to humans in reports, etc.</t>
+  </si>
+  <si>
+    <t>.title</t>
+  </si>
+  <si>
+    <t>FiveWs.what[x]</t>
+  </si>
+  <si>
+    <t>Account.subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">target
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Patient|Device|Practitioner|PractitionerRole|Location|HealthcareService|Organization)
+</t>
+  </si>
+  <si>
+    <t>The entity that caused the expenses</t>
+  </si>
+  <si>
+    <t>Identifies the entity which incurs the expenses. While the immediate recipients of services or goods might be entities related to the subject, the expenses were ultimately incurred by the subject of the Account.</t>
+  </si>
+  <si>
+    <t>Accounts can be applied to non-patients for tracking other non-patient related activities, such as group services (patients not tracked, and costs charged to another body), or might not be allocated.</t>
+  </si>
+  <si>
+    <t>.subject</t>
+  </si>
+  <si>
+    <t>FiveWs.subject</t>
+  </si>
+  <si>
+    <t>Account.servicePeriod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period
+</t>
+  </si>
+  <si>
+    <t>Transaction window</t>
+  </si>
+  <si>
+    <t>The date range of services associated with this account.</t>
+  </si>
+  <si>
+    <t>It is possible for transactions to be posted outside the service period, as long as the service was provided within the defined service period.</t>
+  </si>
+  <si>
+    <t>.coverage.insurancePolicy.effectiveTime</t>
+  </si>
+  <si>
+    <t>FiveWs.done[x]</t>
   </si>
   <si>
     <t>Account.coverage</t>
@@ -375,6 +503,47 @@
     <t>.coverage</t>
   </si>
   <si>
+    <t>Account.coverage.id</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Account.coverage.extension</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>Account.coverage.modifierExtension</t>
+  </si>
+  <si>
+    <t>extensions
+user contentmodifiers</t>
+  </si>
+  <si>
+    <t>Extensions that cannot be ignored even if unrecognized</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element and that modifies the understanding of the element in which it is contained and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
+Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
+  </si>
+  <si>
+    <t>BackboneElement.modifierExtension</t>
+  </si>
+  <si>
     <t>Account.coverage.coverage</t>
   </si>
   <si>
@@ -415,6 +584,22 @@
     <t>.coverage.sequenceNumber</t>
   </si>
   <si>
+    <t>Account.owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Organization)
+</t>
+  </si>
+  <si>
+    <t>Entity managing the Account</t>
+  </si>
+  <si>
+    <t>Indicates the service area, hospital, department, etc. with responsibility for managing the Account.</t>
+  </si>
+  <si>
+    <t>.holder</t>
+  </si>
+  <si>
     <t>Account.description</t>
   </si>
   <si>
@@ -437,6 +622,31 @@
   </si>
   <si>
     <t>.holder.guarantorRole</t>
+  </si>
+  <si>
+    <t>Account.guarantor.id</t>
+  </si>
+  <si>
+    <t>Account.guarantor.extension</t>
+  </si>
+  <si>
+    <t>Account.guarantor.modifierExtension</t>
+  </si>
+  <si>
+    <t>Account.guarantor.party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Patient|RelatedPerson|Organization)
+</t>
+  </si>
+  <si>
+    <t>Responsible entity</t>
+  </si>
+  <si>
+    <t>The entity who is responsible.</t>
+  </si>
+  <si>
+    <t>.holder.guarantorRole[guarantorPerson|guarantorOrganization]</t>
   </si>
   <si>
     <t>Account.guarantor.onHold</t>
@@ -455,29 +665,9 @@
     <t>.holder.guarantorRole.statusCode</t>
   </si>
   <si>
-    <t>Account.guarantor.party</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(Patient|RelatedPerson|Organization)
-</t>
-  </si>
-  <si>
-    <t>Responsible entity</t>
-  </si>
-  <si>
-    <t>The entity who is responsible.</t>
-  </si>
-  <si>
-    <t>.holder.guarantorRole[guarantorPerson|guarantorOrganization]</t>
-  </si>
-  <si>
     <t>Account.guarantor.period</t>
   </si>
   <si>
-    <t xml:space="preserve">Period
-</t>
-  </si>
-  <si>
     <t>Guarantee account during</t>
   </si>
   <si>
@@ -485,60 +675,6 @@
   </si>
   <si>
     <t>.holder.guarantorRole.effectiveTime</t>
-  </si>
-  <si>
-    <t>Account.identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identifier
-</t>
-  </si>
-  <si>
-    <t>Account number</t>
-  </si>
-  <si>
-    <t>Unique identifier used to reference the account.  Might or might not be intended for human use (e.g. credit card number).</t>
-  </si>
-  <si>
-    <t>.id</t>
-  </si>
-  <si>
-    <t>FiveWs.identifier</t>
-  </si>
-  <si>
-    <t>Account.name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title
-</t>
-  </si>
-  <si>
-    <t>Human-readable label</t>
-  </si>
-  <si>
-    <t>Name used for the account when displaying it to humans in reports, etc.</t>
-  </si>
-  <si>
-    <t>.title</t>
-  </si>
-  <si>
-    <t>FiveWs.what[x]</t>
-  </si>
-  <si>
-    <t>Account.owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(Organization)
-</t>
-  </si>
-  <si>
-    <t>Entity managing the Account</t>
-  </si>
-  <si>
-    <t>Indicates the service area, hospital, department, etc. with responsibility for managing the Account.</t>
-  </si>
-  <si>
-    <t>.holder</t>
   </si>
   <si>
     <t>Account.partOf</t>
@@ -552,105 +688,6 @@
   </si>
   <si>
     <t>Reference to a parent Account.</t>
-  </si>
-  <si>
-    <t>Account.servicePeriod</t>
-  </si>
-  <si>
-    <t>Transaction window</t>
-  </si>
-  <si>
-    <t>The date range of services associated with this account.</t>
-  </si>
-  <si>
-    <t>It is possible for transactions to be posted outside the service period, as long as the service was provided within the defined service period.</t>
-  </si>
-  <si>
-    <t>.coverage.insurancePolicy.effectiveTime</t>
-  </si>
-  <si>
-    <t>FiveWs.done[x]</t>
-  </si>
-  <si>
-    <t>Account.status</t>
-  </si>
-  <si>
-    <t>active | inactive | entered-in-error | on-hold | unknown</t>
-  </si>
-  <si>
-    <t>Indicates whether the account is presently used/usable or not.</t>
-  </si>
-  <si>
-    <t>This element is labeled as a modifier because the status contains the codes inactive and entered-in-error that mark the Account as not currently valid.</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>Indicates whether the account is available to be used.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/account-status|4.0.1</t>
-  </si>
-  <si>
-    <t>.statusCode</t>
-  </si>
-  <si>
-    <t>FiveWs.status</t>
-  </si>
-  <si>
-    <t>Account.subject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">target
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(Patient|Device|Practitioner|PractitionerRole|Location|HealthcareService|Organization)
-</t>
-  </si>
-  <si>
-    <t>The entity that caused the expenses</t>
-  </si>
-  <si>
-    <t>Identifies the entity which incurs the expenses. While the immediate recipients of services or goods might be entities related to the subject, the expenses were ultimately incurred by the subject of the Account.</t>
-  </si>
-  <si>
-    <t>Accounts can be applied to non-patients for tracking other non-patient related activities, such as group services (patients not tracked, and costs charged to another body), or might not be allocated.</t>
-  </si>
-  <si>
-    <t>.subject</t>
-  </si>
-  <si>
-    <t>FiveWs.subject</t>
-  </si>
-  <si>
-    <t>Account.type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CodeableConcept
-</t>
-  </si>
-  <si>
-    <t>E.g. patient, expense, depreciation</t>
-  </si>
-  <si>
-    <t>Categorizes the account for reporting and searching purposes.</t>
-  </si>
-  <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>The usage type of this account, permits categorization of accounts.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/account-type</t>
-  </si>
-  <si>
-    <t>.code</t>
-  </si>
-  <si>
-    <t>FiveWs.class</t>
   </si>
 </sst>
 </file>
@@ -799,7 +836,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK26"/>
+  <dimension ref="A1:AK32"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -808,7 +845,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="25.359375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="34.375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
@@ -835,10 +872,10 @@
     <col min="25" max="25" width="45.95703125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="18.84375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="32.79296875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="31" max="31" width="33.4296875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
@@ -1042,7 +1079,7 @@
         <v>41</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="AF2" t="s" s="2">
         <v>39</v>
@@ -1054,7 +1091,7 @@
         <v>41</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AJ2" t="s" s="2">
         <v>37</v>
@@ -1065,7 +1102,7 @@
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -1076,28 +1113,28 @@
         <v>39</v>
       </c>
       <c r="F3" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I3" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="G3" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H3" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I3" t="s" s="2">
+      <c r="J3" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="J3" t="s" s="2">
+      <c r="K3" t="s" s="2">
         <v>49</v>
       </c>
-      <c r="K3" t="s" s="2">
+      <c r="L3" t="s" s="2">
         <v>50</v>
       </c>
-      <c r="L3" t="s" s="2">
+      <c r="M3" t="s" s="2">
         <v>51</v>
-      </c>
-      <c r="M3" t="s" s="2">
-        <v>52</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" t="s" s="2">
@@ -1147,13 +1184,13 @@
         <v>41</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AF3" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH3" t="s" s="2">
         <v>41</v>
@@ -1170,7 +1207,7 @@
     </row>
     <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
@@ -1181,25 +1218,25 @@
         <v>39</v>
       </c>
       <c r="F4" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="G4" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H4" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I4" t="s" s="2">
-        <v>48</v>
-      </c>
       <c r="J4" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="K4" t="s" s="2">
         <v>55</v>
       </c>
-      <c r="K4" t="s" s="2">
+      <c r="L4" t="s" s="2">
         <v>56</v>
-      </c>
-      <c r="L4" t="s" s="2">
-        <v>57</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1250,19 +1287,19 @@
         <v>41</v>
       </c>
       <c r="AE4" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AF4" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG4" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH4" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI4" t="s" s="2">
         <v>58</v>
-      </c>
-      <c r="AF4" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG4" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH4" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI4" t="s" s="2">
-        <v>59</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>41</v>
@@ -1273,7 +1310,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -1284,28 +1321,28 @@
         <v>39</v>
       </c>
       <c r="F5" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G5" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="G5" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H5" t="s" s="2">
-        <v>48</v>
-      </c>
       <c r="I5" t="s" s="2">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J5" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="K5" t="s" s="2">
         <v>61</v>
       </c>
-      <c r="K5" t="s" s="2">
+      <c r="L5" t="s" s="2">
         <v>62</v>
       </c>
-      <c r="L5" t="s" s="2">
+      <c r="M5" t="s" s="2">
         <v>63</v>
-      </c>
-      <c r="M5" t="s" s="2">
-        <v>64</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
@@ -1355,19 +1392,19 @@
         <v>41</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH5" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ5" t="s" s="2">
         <v>41</v>
@@ -1378,7 +1415,7 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -1389,7 +1426,7 @@
         <v>39</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G6" t="s" s="2">
         <v>41</v>
@@ -1401,16 +1438,16 @@
         <v>41</v>
       </c>
       <c r="J6" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="K6" t="s" s="2">
         <v>67</v>
       </c>
-      <c r="K6" t="s" s="2">
+      <c r="L6" t="s" s="2">
         <v>68</v>
       </c>
-      <c r="L6" t="s" s="2">
+      <c r="M6" t="s" s="2">
         <v>69</v>
-      </c>
-      <c r="M6" t="s" s="2">
-        <v>70</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" t="s" s="2">
@@ -1436,43 +1473,43 @@
         <v>41</v>
       </c>
       <c r="W6" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="X6" t="s" s="2">
         <v>71</v>
       </c>
-      <c r="X6" t="s" s="2">
+      <c r="Y6" t="s" s="2">
         <v>72</v>
       </c>
-      <c r="Y6" t="s" s="2">
+      <c r="Z6" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA6" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB6" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC6" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD6" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE6" t="s" s="2">
         <v>73</v>
       </c>
-      <c r="Z6" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA6" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB6" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC6" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD6" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE6" t="s" s="2">
-        <v>74</v>
-      </c>
       <c r="AF6" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH6" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>41</v>
@@ -1483,18 +1520,18 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" t="s" s="2">
         <v>41</v>
@@ -1506,16 +1543,16 @@
         <v>41</v>
       </c>
       <c r="J7" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="K7" t="s" s="2">
         <v>77</v>
       </c>
-      <c r="K7" t="s" s="2">
+      <c r="L7" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="L7" t="s" s="2">
+      <c r="M7" t="s" s="2">
         <v>79</v>
-      </c>
-      <c r="M7" t="s" s="2">
-        <v>80</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
@@ -1565,22 +1602,22 @@
         <v>41</v>
       </c>
       <c r="AE7" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF7" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG7" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH7" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI7" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="AJ7" t="s" s="2">
         <v>81</v>
-      </c>
-      <c r="AF7" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG7" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH7" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI7" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="AJ7" t="s" s="2">
-        <v>82</v>
       </c>
       <c r="AK7" t="s" s="2">
         <v>41</v>
@@ -1588,11 +1625,11 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s" s="2">
@@ -1611,16 +1648,16 @@
         <v>41</v>
       </c>
       <c r="J8" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="K8" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="K8" t="s" s="2">
+      <c r="L8" t="s" s="2">
         <v>86</v>
       </c>
-      <c r="L8" t="s" s="2">
+      <c r="M8" t="s" s="2">
         <v>87</v>
-      </c>
-      <c r="M8" t="s" s="2">
-        <v>88</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -1670,7 +1707,7 @@
         <v>41</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>39</v>
@@ -1685,7 +1722,7 @@
         <v>41</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AK8" t="s" s="2">
         <v>41</v>
@@ -1693,11 +1730,11 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
@@ -1716,16 +1753,16 @@
         <v>41</v>
       </c>
       <c r="J9" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K9" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="K9" t="s" s="2">
+      <c r="L9" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="L9" t="s" s="2">
+      <c r="M9" t="s" s="2">
         <v>95</v>
-      </c>
-      <c r="M9" t="s" s="2">
-        <v>96</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -1763,19 +1800,19 @@
         <v>41</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>97</v>
+        <v>41</v>
       </c>
       <c r="AB9" t="s" s="2">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="AC9" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>39</v>
@@ -1787,10 +1824,10 @@
         <v>41</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AK9" t="s" s="2">
         <v>41</v>
@@ -1798,11 +1835,11 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
@@ -1815,25 +1852,25 @@
         <v>41</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I10" t="s" s="2">
         <v>41</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N10" t="s" s="2">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="O10" t="s" s="2">
         <v>41</v>
@@ -1870,19 +1907,19 @@
         <v>41</v>
       </c>
       <c r="AA10" t="s" s="2">
-        <v>97</v>
+        <v>41</v>
       </c>
       <c r="AB10" t="s" s="2">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="AC10" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD10" t="s" s="2">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>39</v>
@@ -1894,10 +1931,10 @@
         <v>41</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AK10" t="s" s="2">
         <v>41</v>
@@ -1905,7 +1942,7 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -1925,20 +1962,18 @@
         <v>41</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="M11" t="s" s="2">
-        <v>111</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
         <v>41</v>
@@ -1987,7 +2022,7 @@
         <v>41</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>39</v>
@@ -1999,18 +2034,18 @@
         <v>41</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>41</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -2018,30 +2053,32 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G12" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="F12" t="s" s="2">
+      <c r="I12" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="G12" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H12" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I12" t="s" s="2">
-        <v>48</v>
-      </c>
       <c r="J12" t="s" s="2">
-        <v>114</v>
+        <v>66</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="M12" s="2"/>
+        <v>111</v>
+      </c>
+      <c r="M12" t="s" s="2">
+        <v>112</v>
+      </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
         <v>41</v>
@@ -2066,13 +2103,13 @@
         <v>41</v>
       </c>
       <c r="W12" t="s" s="2">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="Z12" t="s" s="2">
         <v>41</v>
@@ -2090,25 +2127,25 @@
         <v>41</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AG12" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH12" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="AJ12" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="AK12" t="s" s="2">
         <v>117</v>
-      </c>
-      <c r="AK12" t="s" s="2">
-        <v>41</v>
       </c>
     </row>
     <row r="13" hidden="true">
@@ -2117,36 +2154,34 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F13" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G13" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I13" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="G13" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H13" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I13" t="s" s="2">
-        <v>48</v>
-      </c>
       <c r="J13" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="K13" t="s" s="2">
         <v>120</v>
       </c>
-      <c r="K13" t="s" s="2">
+      <c r="L13" t="s" s="2">
         <v>121</v>
       </c>
-      <c r="L13" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="M13" t="s" s="2">
-        <v>123</v>
-      </c>
+      <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
         <v>41</v>
@@ -2171,13 +2206,13 @@
         <v>41</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>41</v>
+        <v>122</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>41</v>
+        <v>123</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>41</v>
+        <v>124</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>41</v>
@@ -2201,53 +2236,53 @@
         <v>39</v>
       </c>
       <c r="AG13" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH13" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>41</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>41</v>
+        <v>128</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F14" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G14" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H14" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I14" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="G14" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H14" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I14" t="s" s="2">
+      <c r="J14" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="J14" t="s" s="2">
-        <v>49</v>
-      </c>
       <c r="K14" t="s" s="2">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -2298,34 +2333,34 @@
         <v>41</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG14" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH14" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>41</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>41</v>
+        <v>134</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
@@ -2341,18 +2376,20 @@
         <v>41</v>
       </c>
       <c r="I15" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="M15" s="2"/>
+        <v>137</v>
+      </c>
+      <c r="M15" t="s" s="2">
+        <v>138</v>
+      </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
         <v>41</v>
@@ -2401,7 +2438,7 @@
         <v>41</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>39</v>
@@ -2413,18 +2450,18 @@
         <v>41</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>41</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2435,27 +2472,29 @@
         <v>39</v>
       </c>
       <c r="F16" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G16" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H16" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I16" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="G16" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H16" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I16" t="s" s="2">
-        <v>41</v>
-      </c>
       <c r="J16" t="s" s="2">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="M16" s="2"/>
+        <v>144</v>
+      </c>
+      <c r="M16" t="s" s="2">
+        <v>145</v>
+      </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
         <v>41</v>
@@ -2504,30 +2543,30 @@
         <v>41</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG16" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH16" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>41</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2535,30 +2574,32 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G17" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H17" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I17" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="F17" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G17" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H17" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I17" t="s" s="2">
-        <v>41</v>
-      </c>
       <c r="J17" t="s" s="2">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="M17" s="2"/>
+        <v>151</v>
+      </c>
+      <c r="M17" t="s" s="2">
+        <v>152</v>
+      </c>
       <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
         <v>41</v>
@@ -2607,22 +2648,22 @@
         <v>41</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH17" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="AK17" t="s" s="2">
         <v>41</v>
@@ -2630,7 +2671,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2641,7 +2682,7 @@
         <v>39</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>41</v>
@@ -2653,13 +2694,13 @@
         <v>41</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>144</v>
+        <v>48</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2710,13 +2751,13 @@
         <v>41</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH18" t="s" s="2">
         <v>41</v>
@@ -2725,7 +2766,7 @@
         <v>41</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>41</v>
@@ -2733,11 +2774,11 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -2753,18 +2794,20 @@
         <v>41</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>149</v>
+        <v>92</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>150</v>
+        <v>93</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="M19" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="M19" t="s" s="2">
+        <v>95</v>
+      </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
         <v>41</v>
@@ -2813,7 +2856,7 @@
         <v>41</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>39</v>
@@ -2825,50 +2868,54 @@
         <v>41</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>153</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G20" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H20" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="G20" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H20" t="s" s="2">
-        <v>41</v>
-      </c>
       <c r="I20" t="s" s="2">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
+        <v>165</v>
+      </c>
+      <c r="M20" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="N20" t="s" s="2">
+        <v>101</v>
+      </c>
       <c r="O20" t="s" s="2">
         <v>41</v>
       </c>
@@ -2916,30 +2963,30 @@
         <v>41</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>158</v>
+        <v>89</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>159</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -2947,28 +2994,28 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I21" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="G21" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H21" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I21" t="s" s="2">
-        <v>48</v>
-      </c>
       <c r="J21" t="s" s="2">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -3019,22 +3066,22 @@
         <v>41</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="AG21" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH21" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>41</v>
@@ -3042,38 +3089,40 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>41</v>
+        <v>173</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F22" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G22" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H22" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I22" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="G22" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H22" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I22" t="s" s="2">
-        <v>41</v>
-      </c>
       <c r="J22" t="s" s="2">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="M22" s="2"/>
+        <v>176</v>
+      </c>
+      <c r="M22" t="s" s="2">
+        <v>177</v>
+      </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
         <v>41</v>
@@ -3122,22 +3171,22 @@
         <v>41</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>41</v>
+        <v>178</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>41</v>
@@ -3145,7 +3194,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3156,29 +3205,27 @@
         <v>39</v>
       </c>
       <c r="F23" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G23" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H23" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I23" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="G23" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H23" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I23" t="s" s="2">
-        <v>48</v>
-      </c>
       <c r="J23" t="s" s="2">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>172</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>41</v>
@@ -3227,30 +3274,30 @@
         <v>41</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>174</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3258,32 +3305,30 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F24" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G24" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H24" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I24" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="F24" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G24" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H24" t="s" s="2">
+      <c r="J24" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="I24" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="J24" t="s" s="2">
-        <v>67</v>
-      </c>
       <c r="K24" t="s" s="2">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>178</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
         <v>41</v>
@@ -3308,13 +3353,13 @@
         <v>41</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>179</v>
+        <v>41</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>180</v>
+        <v>41</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>181</v>
+        <v>41</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>41</v>
@@ -3332,34 +3377,34 @@
         <v>41</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG24" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH24" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>183</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>185</v>
+        <v>41</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
@@ -3375,20 +3420,18 @@
         <v>41</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>186</v>
+        <v>149</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="M25" t="s" s="2">
-        <v>189</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
         <v>41</v>
@@ -3437,7 +3480,7 @@
         <v>41</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>39</v>
@@ -3449,13 +3492,13 @@
         <v>41</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>191</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" hidden="true">
@@ -3471,7 +3514,7 @@
         <v>39</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>41</v>
@@ -3480,16 +3523,16 @@
         <v>41</v>
       </c>
       <c r="I26" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J26" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="J26" t="s" s="2">
-        <v>193</v>
-      </c>
       <c r="K26" t="s" s="2">
-        <v>194</v>
+        <v>155</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>195</v>
+        <v>156</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -3516,53 +3559,677 @@
         <v>41</v>
       </c>
       <c r="W26" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X26" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y26" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z26" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA26" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB26" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC26" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD26" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE26" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="AF26" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG26" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH26" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI26" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ26" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="AK26" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" hidden="true">
+      <c r="A27" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J27" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K27" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="L27" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="M27" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="N27" s="2"/>
+      <c r="O27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P27" s="2"/>
+      <c r="Q27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE27" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="AF27" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AH27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI27" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="AJ27" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="AK27" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" hidden="true">
+      <c r="A28" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H28" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="I28" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="J28" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K28" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="L28" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="M28" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="N28" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="O28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P28" s="2"/>
+      <c r="Q28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE28" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="AF28" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AH28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI28" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="AJ28" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="AK28" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" hidden="true">
+      <c r="A29" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="F29" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J29" t="s" s="2">
         <v>196</v>
       </c>
-      <c r="X26" t="s" s="2">
+      <c r="K29" t="s" s="2">
         <v>197</v>
       </c>
-      <c r="Y26" t="s" s="2">
+      <c r="L29" t="s" s="2">
         <v>198</v>
       </c>
-      <c r="Z26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE26" t="s" s="2">
-        <v>192</v>
-      </c>
-      <c r="AF26" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG26" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ26" t="s" s="2">
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P29" s="2"/>
+      <c r="Q29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE29" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="AF29" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI29" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="AK26" t="s" s="2">
+      <c r="AK29" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" hidden="true">
+      <c r="A30" t="s" s="2">
         <v>200</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F30" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J30" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="K30" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="L30" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P30" s="2"/>
+      <c r="Q30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE30" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="AF30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG30" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI30" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="AJ30" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="AK30" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" hidden="true">
+      <c r="A31" t="s" s="2">
+        <v>205</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F31" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J31" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="K31" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="L31" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P31" s="2"/>
+      <c r="Q31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE31" t="s" s="2">
+        <v>205</v>
+      </c>
+      <c r="AF31" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG31" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI31" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="AK31" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" hidden="true">
+      <c r="A32" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F32" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J32" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="K32" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="L32" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P32" s="2"/>
+      <c r="Q32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE32" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="AF32" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG32" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AH32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI32" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="AJ32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK32" t="s" s="2">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK26">
+  <autoFilter ref="A1:AK32">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -3572,7 +4239,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI25">
+  <conditionalFormatting sqref="A2:AI31">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>